<commit_message>
Added optional gene_expr edge annotation and added hra-pop gene expressions to the graph
</commit_message>
<xml_diff>
--- a/schemas/generated/excel/kg.xlsx
+++ b/schemas/generated/excel/kg.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Node" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Edge" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Graph" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Node" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Edge" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Graph" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,11 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>source</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>gene_expr</t>
         </is>
       </c>
     </row>

</xml_diff>